<commit_message>
Colect BSLS MacOS <-> Windows
</commit_message>
<xml_diff>
--- a/keyboards/crkbd/keymaps/ken16itapon/フラグ管理.xlsx
+++ b/keyboards/crkbd/keymaps/ken16itapon/フラグ管理.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\ken16\Documents\qmk_firmware\keyboards\crkbd\keymaps\ken16itapon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A6E8E16-B862-47B5-8ECE-8B2C911C7547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AE36B5-DC45-46C6-AA6A-08FD6C235A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63420" yWindow="9360" windowWidth="23850" windowHeight="18915" xr2:uid="{55139171-E41B-4E64-A1D8-0FFF7CA5C147}"/>
+    <workbookView xWindow="26790" yWindow="4155" windowWidth="29145" windowHeight="18000" activeTab="1" xr2:uid="{55139171-E41B-4E64-A1D8-0FFF7CA5C147}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="86">
   <si>
     <t>単打</t>
     <rPh sb="0" eb="2">
@@ -109,10 +110,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>backspace_sent=true</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -168,6 +165,232 @@
   </si>
   <si>
     <t>lower_holding=false</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state.pressed_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state.released_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state.other_key_pressed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state.bspc_active</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state.backspace_sent</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state.rapid_press</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state.mods_active</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raise_state.pressed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raise_state.pressed_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ime_state.henkan_pressed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ime_state.henkan_pressed_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ime_state.mhenkan_pressed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ime_state.mhenkan_pressed_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ime_state.mods_active</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">lower_state.pressed     </t>
+  </si>
+  <si>
+    <t>KC_LALT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KC_LGUI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?TRUE-&gt;FALSE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?&gt;=T_T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?&lt;T_T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SET</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LAYER(_LOWER)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?&lt;TT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?FALSE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KC_BSPC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LAYER(_RAISE)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>!LOWER=PRESSED</t>
+  </si>
+  <si>
+    <t>?LOWER=PRESSED</t>
+  </si>
+  <si>
+    <t>?RAISE=PRESSED</t>
+  </si>
+  <si>
+    <t>?LOWER=RELEASED</t>
+  </si>
+  <si>
+    <t>?RAISE=RELEASED</t>
+  </si>
+  <si>
+    <t>_=RELEASED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lower_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pressed     </t>
+  </si>
+  <si>
+    <t>pressed_time</t>
+  </si>
+  <si>
+    <t>released_time</t>
+  </si>
+  <si>
+    <t>other_key_pressed</t>
+  </si>
+  <si>
+    <t>bspc_active</t>
+  </si>
+  <si>
+    <t>backspace_sent</t>
+  </si>
+  <si>
+    <t>rapid_press</t>
+  </si>
+  <si>
+    <t>mods_active</t>
+  </si>
+  <si>
+    <t>raise_state</t>
+  </si>
+  <si>
+    <t>pressed</t>
+  </si>
+  <si>
+    <t>ime_state</t>
+  </si>
+  <si>
+    <t>henkan_pressed</t>
+  </si>
+  <si>
+    <t>henkan_pressed_time</t>
+  </si>
+  <si>
+    <t>mhenkan_pressed</t>
+  </si>
+  <si>
+    <t>mhenkan_pressed_time</t>
+  </si>
+  <si>
+    <t>KC_SPC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TRUE-&gt;FALSE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?MHENKAN=PRESSED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?MHENKAN=RELEASED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HENKAN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MHENKAN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TAP</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NAGINATA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OFF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?HENKAN=PRESSED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>?HENKAN=RELEASED</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ON</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BIT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -210,12 +433,173 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -224,7 +608,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -233,6 +617,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,12 +995,41 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="567" row="15">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{74B6332E-77E6-48B0-B4B2-868A030D11D5}">
+  <we:reference id="81ae7f57-2760-4043-a9cb-e0d36209e808" version="1.3.0.0" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences>
+    <we:reference id="WA200003696" version="1.3.0.0" store="ja-JP" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{9CF5B33D-63AB-4BE2-94A4-3F60CB878620}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3847CA-A00A-4791-B396-3D9CB4AE5429}">
-  <dimension ref="A3:H32"/>
+  <dimension ref="A3:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,25 +1043,25 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -622,7 +1080,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -630,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -642,12 +1100,12 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>1</v>
@@ -656,46 +1114,46 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>2</v>
       </c>
@@ -703,17 +1161,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
@@ -723,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>1</v>
       </c>
@@ -731,7 +1189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>8</v>
       </c>
@@ -742,13 +1200,954 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>11</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084FBE35-D467-45EB-B72E-5426509A2E66}">
+  <dimension ref="A1:Q34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="13.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="15" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="11"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="14"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q14" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q15" s="11"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="11"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="11"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="14"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAFkATQBEACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgClACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGoAYQAtAGoAcAAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CF5B33D-63AB-4BE2-94A4-3F60CB878620}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>